<commit_message>
Improve formatting of mail merge / pdf
</commit_message>
<xml_diff>
--- a/ProgramPlanning.Web/Learning Outcomes.xlsx
+++ b/ProgramPlanning.Web/Learning Outcomes.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20350"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20351"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ProgramPlanning\ProgramPlanning.Wpf\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ProgramPlanning\ProgramPlanning.Web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08137168-8772-4CE0-8333-062C90CB003C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CFB07F5-13BD-4309-B173-036A4F1C6BC5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="14100" xr2:uid="{736E1BEA-C0B9-40DD-8022-BD2245546042}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="0" r:id="rId3"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="225">
   <si>
     <t>Course</t>
   </si>
@@ -735,6 +739,18 @@
   </si>
   <si>
     <t>Advanced Algorithms</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Column Labels</t>
+  </si>
+  <si>
+    <t>Count of ItemText</t>
   </si>
 </sst>
 </file>
@@ -770,11 +786,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -790,6 +814,1953 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Jonathan Allen" refreshedDate="43773.621688657404" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="261" xr:uid="{5518AC90-624F-4DFA-B980-7B7BBF4E4D4E}">
+  <cacheSource type="worksheet">
+    <worksheetSource name="Table1"/>
+  </cacheSource>
+  <cacheFields count="4">
+    <cacheField name="Area" numFmtId="0">
+      <sharedItems count="8">
+        <s v="COMM"/>
+        <s v="CS"/>
+        <s v="ENGL"/>
+        <s v="GE"/>
+        <s v="MAT/SCI"/>
+        <s v="MATH"/>
+        <s v="PHYS"/>
+        <s v="SE"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Course" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="4450" count="44">
+        <n v="1020"/>
+        <n v="1400"/>
+        <n v="1405"/>
+        <n v="1410"/>
+        <n v="1415"/>
+        <n v="1810"/>
+        <n v="1820"/>
+        <n v="2420"/>
+        <n v="2450"/>
+        <n v="2700"/>
+        <n v="2810"/>
+        <n v="2830"/>
+        <n v="2860"/>
+        <n v="1010"/>
+        <n v="2010"/>
+        <n v="3260"/>
+        <n v="1"/>
+        <n v="2"/>
+        <n v="3"/>
+        <n v="4"/>
+        <n v="5"/>
+        <n v="1210"/>
+        <n v="1220"/>
+        <n v="2270"/>
+        <n v="3040"/>
+        <n v="3310"/>
+        <n v="2210"/>
+        <n v="2215"/>
+        <n v="2220"/>
+        <n v="2225"/>
+        <n v="3250"/>
+        <n v="3410"/>
+        <n v="3450"/>
+        <n v="3520"/>
+        <n v="3620"/>
+        <n v="3630"/>
+        <n v="4120"/>
+        <n v="4140"/>
+        <n v="4220"/>
+        <n v="4230"/>
+        <n v="4320"/>
+        <n v="4340"/>
+        <n v="4400"/>
+        <n v="4450"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="ItemType" numFmtId="0">
+      <sharedItems count="6">
+        <s v="Title"/>
+        <s v="Semester"/>
+        <s v="Learning Outcome"/>
+        <s v="Content"/>
+        <s v="Prereq"/>
+        <s v="Coreq"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="ItemText" numFmtId="0">
+      <sharedItems longText="1"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="261">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Communications (?)"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="Yr4 - Spring"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="2"/>
+    <s v="Students will know the basic data types, control structures, and programming approaches for a current programming language.  "/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="2"/>
+    <s v="Students will be able to solve problems by developing algorithms and implementing those algorithms using a current programming language."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="2"/>
+    <s v="Students will begin to understand the social responsibilities of the computing professional and the impact of computing on society"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="3"/>
+    <s v="The following topics will be covered in this course: Introduction to computers and programming; Data representation; Control structures; Functions; Arrays; Social context of computing."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="Programming Fundamentals"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <s v="Prerequisites"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="1"/>
+    <s v="Prerequisites"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="2"/>
+    <s v="Students will know some basic data structures, basic software methodologies, and machine level representation of data."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="2"/>
+    <s v="Students will be able to apply appropriate software design methodologies for larger programs, use appropriate data structures, and use an object-oriented language."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="3"/>
+    <s v="The following topics will be covered in this course: Encapsulation; Inheritance; Polymorphism; Exception handling. Basic data structures; Recursion; The software development process"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="0"/>
+    <s v="Object-Oriented Programming"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="4"/>
+    <s v="CS 1400"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="5"/>
+    <s v="CS 1415"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="1"/>
+    <s v="Yr1 - Fall"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="4"/>
+    <x v="1"/>
+    <s v="Yr1 - Fall"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="2"/>
+    <s v="Students will be able to build a simple web site that organizes information effectively"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="2"/>
+    <s v="Students will be able to identify an organization for information based on its inherent structure (chronological, alphabetic, etc.)."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="2"/>
+    <s v="Students will be able to use cascading style sheets to create style standards for a web site."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="2"/>
+    <s v="Students will be able to create a navigational framework that matches the content and genre of the site."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="2"/>
+    <s v="Students will be able to explain separation of concerns as it applies to the design and implementation of a web site"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="2"/>
+    <s v="Students will be able to describe the issues involved in developing a web interface."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="2"/>
+    <s v="Students will be able to summarize the need and issues involved in web site implementation and integration."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="2"/>
+    <s v="Students will be able to explain why accessibility issues are an important consideration in web page development."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="2"/>
+    <s v="Students will be able to design and implement a web interface"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="2"/>
+    <s v="Students will be able to compare/contrast graphic media file format characteristics such as color depth, compression and CODEC"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="2"/>
+    <s v="Students will be able to explain and compare media file formats including lossy vs. lossless compression, color palettes, streaming formats, and CODECs"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="2"/>
+    <s v="Students will be able to explain and compare the inter-operability of formats"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="3"/>
+    <s v="The course provides a technical overview of the Internet environment and the structure of the World Wide Web. The technical segment will focus on the design and implementation of an effective web site at the introductory level."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="0"/>
+    <s v="Web Development I"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="4"/>
+    <s v="CS 1410"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="1"/>
+    <s v="Yr3 - Fall"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="6"/>
+    <x v="2"/>
+    <s v="Demonstrate how server-side technology works."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="6"/>
+    <x v="2"/>
+    <s v="Develop with server-side technology. Complicated web development environments such as ASP.NET and PHP have a fairly substantial learning curve."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="6"/>
+    <x v="2"/>
+    <s v="Utilize databases in web applications."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="6"/>
+    <x v="2"/>
+    <s v="Implement common data models used in blogs, forums, and content management systems."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="6"/>
+    <x v="2"/>
+    <s v="Design software for web applications. This includes layered software architectures as well as tiered designs for scalability and reliability."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="6"/>
+    <x v="2"/>
+    <s v="Identify mechanisms for maintaining state in web applications. This is one of the most important topics in the course since it is the principal difference between web application development and non-web application development."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="6"/>
+    <x v="2"/>
+    <s v="Consume REST and SOAP web services."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="6"/>
+    <x v="2"/>
+    <s v="Design and implementing web security."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="6"/>
+    <x v="3"/>
+    <s v="CS 1820 introduces the principles of back end web development. The backend of a web application is an enabler for a front end experience. Backend developers need to understand programming languages and database and they must have an understanding of server architecture."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="6"/>
+    <x v="0"/>
+    <s v="Web Development II"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="6"/>
+    <x v="4"/>
+    <s v="CS 1810"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="6"/>
+    <x v="1"/>
+    <s v="Yr3 - Spring"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="7"/>
+    <x v="2"/>
+    <s v="Students will know many basic data structures, recursion, complexity analysis, and common sorting and searching algorithms."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="7"/>
+    <x v="2"/>
+    <s v="Students will be able to use appropriate data structures and data abstraction. They will be able to use recursion as a problem solving strategy. They will be able to analyze complexity of algorithms and use appropriate sorting and searching algorithms."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="7"/>
+    <x v="3"/>
+    <s v="The following topics will be covered in this course: Data abstration; Linked lists; Stacks and queues; Trees; Tables; Graphs; Recursion; Complexity analysis; Sorting and searching"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="7"/>
+    <x v="2"/>
+    <s v="Students will know many basic data structures, recursion, complexity analysis, and common sorting and searching algorithms."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="7"/>
+    <x v="2"/>
+    <s v="Students will be able to use appropriate data structures and data abstraction. They will be able to use recursion as a problem solving strategy. They will be able to analyze complexity of algorithms and use appropriate sorting and searching algorithms."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="7"/>
+    <x v="3"/>
+    <s v="The following topics will be covered in this course: Data abstration; Linked lists; Stacks and queues; Trees; Tables; Graphs; Recursion; Complexity analysis; Sorting and searching"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="7"/>
+    <x v="0"/>
+    <s v="Data Structures and Algorithms"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="7"/>
+    <x v="4"/>
+    <s v="CS 1410"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="7"/>
+    <x v="1"/>
+    <s v="Yr1 - Spring"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="8"/>
+    <x v="2"/>
+    <s v="Underststand software engineering principles."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="8"/>
+    <x v="2"/>
+    <s v="Specify and manage software project requirements."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="8"/>
+    <x v="2"/>
+    <s v="Perform basic software project management."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="8"/>
+    <x v="2"/>
+    <s v="Understand the impact of alternative software development practices like extreme programming (XP) and Agile."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="8"/>
+    <x v="2"/>
+    <s v="Perform unit testing of software."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="8"/>
+    <x v="2"/>
+    <s v="Create work product documentation."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="8"/>
+    <x v="2"/>
+    <s v="Perform project risk management."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="8"/>
+    <x v="2"/>
+    <s v="Work as an effective member of a software development team."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="8"/>
+    <x v="3"/>
+    <s v="The following topics will be covered in this course: Software life cycle models; Software project management; Team development environments and methodologies; Requirements engineering; Software design and architectures; Quality assurance and standards; Legal and ethical issues; Working as an effective member of a software development team"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="8"/>
+    <x v="0"/>
+    <s v="Intro to Software Engineering"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="8"/>
+    <x v="4"/>
+    <s v="CS 2420"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="8"/>
+    <x v="1"/>
+    <s v="Yr2 - Spring"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="9"/>
+    <x v="1"/>
+    <s v="Yr1 - Spring"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="10"/>
+    <x v="2"/>
+    <s v="Students will understand characteristics of an instruction set architecture, an assembly language, assembly level machine organization, and performance and compilation issues."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="10"/>
+    <x v="2"/>
+    <s v="Students will be able to analyze computer system organization at the assembly language level, implement algorithms in assembly/machine language, and design a computer system at a block level."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="10"/>
+    <x v="3"/>
+    <s v="The following topics will be covered in this course: Role of performance; Instruction sets and types; Assembly/machine language; Arithmetic; Datapath and control; Pipelining; Memory management; Interfacing and communication."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="10"/>
+    <x v="0"/>
+    <s v="Computer Organization and Architecture"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="10"/>
+    <x v="4"/>
+    <s v="CS 2420"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="10"/>
+    <x v="1"/>
+    <s v="Yr2 - Fall"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="11"/>
+    <x v="2"/>
+    <s v="Students will be able to employ the public infrastructure as a Service (IaaS) cloud known as Amazon Web Services (AWS) to deploy an existing computer application using cloud computing technologies such as load balancing and auto-scaling."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="11"/>
+    <x v="2"/>
+    <s v="Students will be able to, as part of application deployment, use security controls and technologies available in AWS such as identity and access management, virtual private clouds, security groups, etc."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="11"/>
+    <x v="2"/>
+    <s v="Students will be able to appraise the usefulness of the above-mentioned controls and technologies in terms of relevan security principles and / or attach methods."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="11"/>
+    <x v="2"/>
+    <s v="Students will be able to understand the considerations of architecting a cloud solution."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="11"/>
+    <x v="2"/>
+    <s v="Students will be able to compare and contrast public IaaS with other cloud technologies and models, particularly with respect to resource requirements and security issues."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="11"/>
+    <x v="3"/>
+    <s v="The following topics will be covered in this course: - Introduction to Cloud Computing - Methods of Leveraging Cloud Computing - Cloud Economics and Total Cost of Ownership - AWS Infrastructure - AWS Compute, Storage, and Networking - AWS Security, Identity and Access Management - AWS Database Options - AWS Elasticity and Management Tools - Architecting on AWS and System Design - Methods of Designing Your Environment - System Design for High Availability - Automation and Serverless Architecture - Event-Driven Scaling"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="11"/>
+    <x v="0"/>
+    <s v="Web Development III"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="11"/>
+    <x v="4"/>
+    <s v="CS 1820"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="11"/>
+    <x v="1"/>
+    <s v="Yr4 - Fall"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="12"/>
+    <x v="2"/>
+    <s v="Mechanisms and policies that enable the efficient illusion of concurrent execution of multiple programs upon one (or more) CPUs."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="12"/>
+    <x v="2"/>
+    <s v="Mechanisms and policies that enable a &quot;virtual&quot; address spaces that may be larger than allocated memory."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="12"/>
+    <x v="2"/>
+    <s v="Security mechanisms and policies that protect processes from unauthorized access to their memory or files."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="12"/>
+    <x v="2"/>
+    <s v="Data structures and algorithms used to organize persistent storage."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="12"/>
+    <x v="2"/>
+    <s v="How resources such as CPU time, memory, and persistent storage are managed and allocated."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="12"/>
+    <x v="2"/>
+    <s v="Challenges in concurrency and approaches to avoiding race conditions and deadlock."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="12"/>
+    <x v="2"/>
+    <s v="The intertwined role of interrupts, traps, paged and segmented memory translation, and supervisor mode in enabling multi-tasking, isolation, system calls, access to i/o devices, and timers."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="12"/>
+    <x v="2"/>
+    <s v="Coarse estimations of access time to persistent storage."/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="12"/>
+    <x v="3"/>
+    <s v="This course will cover the following topics: Operating systems history and architecture; Processes and Threads; Synchronization (mostly deadlock prevention); Memory Management; Input/Output; File Systems; Multimedia"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="12"/>
+    <x v="0"/>
+    <s v="Operating Systems"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="12"/>
+    <x v="4"/>
+    <s v="CS 2810"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="12"/>
+    <x v="1"/>
+    <s v="Yr2 - Spring"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="13"/>
+    <x v="0"/>
+    <s v="Composition"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="13"/>
+    <x v="1"/>
+    <s v="Yr1 - Fall"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="14"/>
+    <x v="0"/>
+    <s v="Research Writing"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="14"/>
+    <x v="4"/>
+    <s v="ENGL 1010"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="14"/>
+    <x v="1"/>
+    <s v="Yr1 - Spring"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="15"/>
+    <x v="0"/>
+    <s v="Technical Communications"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="15"/>
+    <x v="4"/>
+    <s v="ENGL 2010"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="15"/>
+    <x v="1"/>
+    <s v="Yr3 - Spring"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="16"/>
+    <x v="0"/>
+    <s v="Life Science"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="17"/>
+    <x v="0"/>
+    <s v="American Institutions"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="17"/>
+    <x v="1"/>
+    <s v="Yr1 - Spring"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="18"/>
+    <x v="0"/>
+    <s v="FA/HU/SS"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="18"/>
+    <x v="1"/>
+    <s v="Yr2 - Fall"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="19"/>
+    <x v="0"/>
+    <s v="FA/HU/SS"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="19"/>
+    <x v="1"/>
+    <s v="Yr2 - Spring"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="20"/>
+    <x v="0"/>
+    <s v="FA/HU/SS"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="20"/>
+    <x v="1"/>
+    <s v="Yr3 - Spring"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="16"/>
+    <x v="0"/>
+    <s v="Elective"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="16"/>
+    <x v="1"/>
+    <s v="Yr2 - Spring"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="21"/>
+    <x v="0"/>
+    <s v="Calc I"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="21"/>
+    <x v="1"/>
+    <s v="Yr1 - Fall"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="21"/>
+    <x v="0"/>
+    <s v="Calc II"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="22"/>
+    <x v="4"/>
+    <s v="MATH 1210"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="22"/>
+    <x v="1"/>
+    <s v="Yr1 - Spring"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="23"/>
+    <x v="0"/>
+    <s v="Linear Algebra"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="23"/>
+    <x v="4"/>
+    <s v="MATH 1210"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="23"/>
+    <x v="1"/>
+    <s v="Yr2 - Fall"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="24"/>
+    <x v="0"/>
+    <s v="Stats for Science &amp; Engineers"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="24"/>
+    <x v="4"/>
+    <s v="MATH 1210"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="24"/>
+    <x v="1"/>
+    <s v="Yr3 - Fall"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="25"/>
+    <x v="0"/>
+    <s v="Discrete"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="25"/>
+    <x v="4"/>
+    <s v="MATH 1210"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="25"/>
+    <x v="1"/>
+    <s v="Yr2 - Fall"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="26"/>
+    <x v="0"/>
+    <s v="Physics for Science &amp; Engineers I"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="26"/>
+    <x v="1"/>
+    <s v="Yr2 - Fall"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="27"/>
+    <x v="0"/>
+    <s v="Physics Lab"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="27"/>
+    <x v="1"/>
+    <s v="Yr2 - Fall"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="28"/>
+    <x v="0"/>
+    <s v="Physics for Science &amp; Engineers II"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="28"/>
+    <x v="4"/>
+    <s v="PHYS 2210"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="28"/>
+    <x v="1"/>
+    <s v="Yr2 - Spring"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="29"/>
+    <x v="0"/>
+    <s v="Physics Lab"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="29"/>
+    <x v="1"/>
+    <s v="Yr2 - Spring"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="30"/>
+    <x v="0"/>
+    <s v="Survey of Languages"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="30"/>
+    <x v="4"/>
+    <s v="CS 2420"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="30"/>
+    <x v="2"/>
+    <s v="Understand the tradeoffs between, use cases for, and theory behind different types of programming languages."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="30"/>
+    <x v="2"/>
+    <s v="Feel comfortable with their ability to learn and use unfamiliar programming languages."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="30"/>
+    <x v="2"/>
+    <s v="Be exposed to and implement programs in a wide variety of programming languages that are used in the software industry."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="30"/>
+    <x v="3"/>
+    <s v="This course will be divided into modules each covering a family of programming languages. In each module, the students will be introduced to a family of languages. We will discuss the use cases and thought patterns that the languages address. Additionally, for each module the students will be expected to learn to develop and debug in a representative language from the family being studied and complete a project using it. This course will cover the following modules: Functional Programming Haskell Interpreted Languages / Scripting Python Declarative Languages Prolog Big data Hadoop/Pig Latin Microsoft .Net C# In addition to the above modules the students will be expected to complete a final project and presentation which will consist of learning a language of their choice, completing a project in that language, and giving a short presentation to the class."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="30"/>
+    <x v="1"/>
+    <s v="Yr3 - Fall"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="31"/>
+    <x v="2"/>
+    <s v="Gather useful information about users and activities through asking, looking, learning, and experimenting with alternatives."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="31"/>
+    <x v="2"/>
+    <s v="Organize information about users into useful summaries with affinity diagrams."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="31"/>
+    <x v="2"/>
+    <s v="Convey user research findings with personas and scenarios."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="31"/>
+    <x v="2"/>
+    <s v="Learn and appreciate the skill of sketching as a process for user experience design."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="31"/>
+    <x v="2"/>
+    <s v="Learn to give and accept critiques of design ideas in a constructive manner."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="31"/>
+    <x v="2"/>
+    <s v="Demonstrate skills for low-fidelity prototyping and describe the strengths and weaknesses of a variety of prototyping methods."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="31"/>
+    <x v="2"/>
+    <s v="Appreciate the process of user experience design as a cyclical, iterative process."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="31"/>
+    <x v="2"/>
+    <s v="Understand the differences between usability and user experience."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="31"/>
+    <x v="2"/>
+    <s v="Analyze an interaction design problem and propose a user-centered process, justifying the process and identifying the trade-offs."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="31"/>
+    <x v="2"/>
+    <s v="Prepare high quality professional documentation and artifacts relating to the design process for preparation for a professional portfolio."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="31"/>
+    <x v="3"/>
+    <s v="SE 3410 introduces the principles of user interface development, focusing on the following areas: • Design: We will look at how to design good user interfaces, covering important design principles (learnability, visibility, error prevention, efficiency, and graphic design) and the human capabilities that motivate them (including perception, motor skills, color vision, attention, and human error). • Implementation: We will see techniques for building user interfaces, including lowfidelity prototypes, Wizard of Oz, and other prototyping tools; input models, output models, model-view-controller, layout, constraints, and toolkits. • Evaluation: We will learn techniques for evaluating and measuring interface usability, including heuristic evaluation, predictive evaluation, and user testing. • Research: We will learn how to conduct empirical research involving novel user interfaces."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="31"/>
+    <x v="0"/>
+    <s v="Human Factors in Software Design"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="31"/>
+    <x v="4"/>
+    <s v="CS 2450"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="31"/>
+    <x v="1"/>
+    <s v="Yr3 - Fall"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="32"/>
+    <x v="2"/>
+    <s v="Demonstrated use of design patterns to reinforce design principles."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="32"/>
+    <x v="2"/>
+    <s v="Developed vocabulary of object-oriented design patterns and principles."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="32"/>
+    <x v="2"/>
+    <s v="Awareness of increase ability to create quality software."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="32"/>
+    <x v="3"/>
+    <s v="The discipline of Software Engineering Design will be presented by covering the following topics: • Software Design processes • Software product design • Product design analysis • Software Engineering Design • Engineering Design • Architectural Design • Object Oriented Design • State Based Design • Patterns in Software Design"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="32"/>
+    <x v="0"/>
+    <s v="Principles and Patterns of Software Design"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="32"/>
+    <x v="4"/>
+    <s v="CS 2450"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="32"/>
+    <x v="1"/>
+    <s v="Yr3 - Spring"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="33"/>
+    <x v="2"/>
+    <s v="Students will learn the techniques and tools to design, guild, and extract information from a database."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="33"/>
+    <x v="2"/>
+    <s v="Understand database design and the use of databases in applications."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="33"/>
+    <x v="2"/>
+    <s v="Understand the relational model, relational algebra, and SQL."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="33"/>
+    <x v="2"/>
+    <s v="Utilize database design and relational design principles based on dependencies and normal forms."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="33"/>
+    <x v="2"/>
+    <s v="Analyze complex business scenarios and create data models"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="33"/>
+    <x v="2"/>
+    <s v="Implement their database design by creating a physical database using SQL"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="33"/>
+    <x v="2"/>
+    <s v="Successfully implement indexes, views, transaction and integrity constraints."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="33"/>
+    <x v="2"/>
+    <s v="Successfully deliver a project which explores database design and management in web applications by utilizing appropriate features of SQL."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="33"/>
+    <x v="3"/>
+    <s v="The following topics will be covered in this course: • Foundations • Design Theory and Constraints • Transactions • Introduction to Database Systems • Specialized and New Data Processing Systems"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="33"/>
+    <x v="0"/>
+    <s v="Database Systems"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="33"/>
+    <x v="4"/>
+    <s v="CS 2420"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="33"/>
+    <x v="1"/>
+    <s v="Yr3 - Fall"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="34"/>
+    <x v="2"/>
+    <s v="Students will demonstrate understanding of distributed operating system and network protocols for process communication, synchronization, scheduling, exception and deadlock resolution."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="34"/>
+    <x v="2"/>
+    <s v="Students will demonstrate via use their understanding of client-server, web-based collaborative systems."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="34"/>
+    <x v="2"/>
+    <s v="Students will demonstrate understanding of parallel computing."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="34"/>
+    <x v="2"/>
+    <s v="Students will demonstrate their ability to solve concurrency issues."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="34"/>
+    <x v="2"/>
+    <s v="Students will exercise API's for distributed application development."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="34"/>
+    <x v="3"/>
+    <s v="Learn and experiment with Amazon Web Services (AWS): • console management • host a static website • build a web application • deploy a web application Understand distributed system components: • distributed system characteristics • system models • networking / internetworking • IPC / RPC • distributed objects • web services • peer to peer • security • distributed file systems • name services • time • transactions and concurrency control • replication"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="34"/>
+    <x v="0"/>
+    <s v="Distributed Application Development"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="34"/>
+    <x v="4"/>
+    <s v="SE 3520"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="34"/>
+    <x v="4"/>
+    <s v="CS 2860"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="34"/>
+    <x v="1"/>
+    <s v="Yr3 - Spring"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="35"/>
+    <x v="2"/>
+    <s v="Students will become familiar with a mobile applications development environment and life cycle. They will know the basics of the Android environment, tools for creating Android applications, the Android approach to structuring applications, basic user interfaces, and the application life cycle."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="35"/>
+    <x v="2"/>
+    <s v="Students will be able to design, implement, test, and debug mobile applications."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="35"/>
+    <x v="3"/>
+    <s v="The following topics will be covered in this course: • Android App Development Tools • Creating and Debugging User Interfaces • User Interace Layouts • Activities and Navigation • Listviews • Input Controls • Multimedia: Android Media Player / Movies and Music • Geolocation: Mapping and location-based services • App Publishing / Content providers • Testing Strategies for Mobile Applications"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="35"/>
+    <x v="0"/>
+    <s v="Mobile Application Development"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="35"/>
+    <x v="4"/>
+    <s v="CS 2420"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="35"/>
+    <x v="1"/>
+    <s v="Yr3 - Spring"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="36"/>
+    <x v="2"/>
+    <s v="Students will be able to write a software project management plan, addressing issues of risk analysis, schedule, costs, team organization, resources, and technical approach."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="36"/>
+    <x v="2"/>
+    <s v="Students will be able to define the technology and practices associated with each and a variety of software development life cycle models and explain the strengths, weaknesses, and applicability of each."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="36"/>
+    <x v="2"/>
+    <s v="Students will be able to define the relationship between software products and overall products (if embedded), or the role of the product in the organizational product line."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="36"/>
+    <x v="2"/>
+    <s v="Students will be able to explain the purpose and limitations of software development standards and be able to apply sensible tailoring where needed."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="36"/>
+    <x v="2"/>
+    <s v="Students will be able to utilize software development standards for documentation and implementation."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="36"/>
+    <x v="2"/>
+    <s v="Students will be able to apply leadership principles to project management."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="36"/>
+    <x v="3"/>
+    <s v="This course covers the following topics: * Life cycle models * Requirements elicitation * Configuration control * Environments * Quality assurance"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="36"/>
+    <x v="0"/>
+    <s v="Management of Software Projects"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="36"/>
+    <x v="4"/>
+    <s v="SE 3410"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="36"/>
+    <x v="1"/>
+    <s v="Yr4 - Fall"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="37"/>
+    <x v="2"/>
+    <s v="Students will understand the connections and interactions between science, technology and society."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="37"/>
+    <x v="2"/>
+    <s v="Students will understand current Intellectual Property debates and the relevant laws governing them."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="37"/>
+    <x v="2"/>
+    <s v="Students will understand privacy concerns posed by modern information gathering methods."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="37"/>
+    <x v="2"/>
+    <s v="Students will be exposed to industry standard codes of ethics put out by ACM and IEEE."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="37"/>
+    <x v="2"/>
+    <s v="Students will understand the history of computing and their place in it."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="37"/>
+    <x v="2"/>
+    <s v="Students will be exposed to philosophical bases for evaluating computer ethics."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="37"/>
+    <x v="3"/>
+    <s v="This course will cover the following modules:_x000a_- History of the rapid rise in computer and networking technology._x000a_- Ethics including an introduction to the philosophical bases._x000a_- Networking and the Internet including Freedom of expression, Censorship, Spam, and_x000a_internet addiction._x000a_- Intellectual Property including copyright, fair use, patents, open-source, and licencing._x000a_- Privacy including the ownership of information, government surveillance, data mining_x000a_and identify theft._x000a_- Computer and Network Security including Viruses, Hackers, and Denial-of-service_x000a_attacks._x000a_- Computer Reliability including the cost and responsibility of errors, software_x000a_warranties, and simulations._x000a_- Professional Ethics including ACM and IEEE codes of conduct."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="37"/>
+    <x v="0"/>
+    <s v="Social and Ethical Issues in Computing"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="37"/>
+    <x v="4"/>
+    <s v="SE 3410"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="37"/>
+    <x v="1"/>
+    <s v="Yr4 - Spring"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="38"/>
+    <x v="2"/>
+    <s v="Students will be able to recognize and use common GUI framework elements, patterns, and concepts."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="38"/>
+    <x v="2"/>
+    <s v="Students will know a modern GUI framework and be comfortable working within it."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="38"/>
+    <x v="2"/>
+    <s v="Students will be familiar with testing and validation strategies for UI frameworks including unit testing, integration testing, and end to end testing."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="38"/>
+    <x v="3"/>
+    <s v="This course will cover the following modules:_x000a_GUI Design and usability_x000a_- This module will cover basic UI/UX considerations including: Discoverability, Error_x000a_prevention, visibility, efficiency, perception, and navigation._x000a_Interaction between front and backend code_x000a_- In this module we will discuss common methods allowing interaction between GUI_x000a_elements and the backend code of an application. These will include events, bindings,_x000a_and MVC patterns._x000a_Layout Tools_x000a_- This module will focus on tools and patterns for laying out UI elements on the screen._x000a_These include grids, canvas, panels, and wrapper elements._x000a_Input_x000a_- This module will focus on getting input from the user. Methods that we will cover include_x000a_buttons, forms, mouse events, keyboard events, drag and drop events, and use of the_x000a_clipboard._x000a_Styles and Themes_x000a_- This module will introduce reusable components for adjusting the visual aspects of the_x000a_interface._x000a_Resources and localization_x000a_- In this module we will discuss methods for creating international applications including_x000a_localization (currency's, date formats, etc.) and languages."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="38"/>
+    <x v="0"/>
+    <s v="Graphical User Interfaces"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="38"/>
+    <x v="4"/>
+    <s v="SE 3250"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="38"/>
+    <x v="4"/>
+    <s v="CS 2450"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="38"/>
+    <x v="1"/>
+    <s v="Yr4 - Fall"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="39"/>
+    <x v="2"/>
+    <s v="Students will be able to design algorithms to solve a variety of computational problems. They will be able to employ any of the following techniques: divide-and-conquer, dynamic programming, greedy approaches, and graph algorithms."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="39"/>
+    <x v="2"/>
+    <s v="Students will be able to analytically reason about and prove the correctness/incorrectness and complexity of algorithmic solutions to problems."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="39"/>
+    <x v="2"/>
+    <s v="Students will be able to implement algorithms in software."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="39"/>
+    <x v="2"/>
+    <s v="Students will be able to reason about the computational complexity of a computation problem by reduction to other problems."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="39"/>
+    <x v="3"/>
+    <s v="Algorithmic techniques will include divide-and-conquer, dynamic programming, greedy approaches, and graph algorithms as well as a selection of current algorithm topics of interest (e.g. learning algorithms). Analysis techniques will include the Master theorem, big-O/theta notation, and proofs by construction, contradiction and induction. Students will also practice implementing algorithms."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="39"/>
+    <x v="0"/>
+    <s v="Advanced Algorithms"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="39"/>
+    <x v="4"/>
+    <s v="MATH 3310"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="39"/>
+    <x v="4"/>
+    <s v="CS 2420"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="39"/>
+    <x v="1"/>
+    <s v="Yr4 - Spring"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="40"/>
+    <x v="2"/>
+    <s v="Students will demonstrate an ability to reduce overall software development defect rates."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="40"/>
+    <x v="2"/>
+    <s v="Students will demonstrate the importance of the time spent at the front end of the development cycle to lay the foundation for a successful project."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="40"/>
+    <x v="2"/>
+    <s v="Students will demonstrate an ability to eliminate or nearly eliminate compile and test defects."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="40"/>
+    <x v="2"/>
+    <s v="Students will be able to accurately estimate the time requirements to build software."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="40"/>
+    <x v="3"/>
+    <s v="The course will cover the following topics:_x000a_- The value of following defined processes._x000a_- Data collection and analysis for continuous improvement of the software development_x000a_life cycle._x000a_- Estimation and planning techniques of software projects._x000a_- Quality management and design principles."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="40"/>
+    <x v="0"/>
+    <s v="Personal Software Practices"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="40"/>
+    <x v="4"/>
+    <s v="SE 3450"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="40"/>
+    <x v="1"/>
+    <s v="Yr4 - Fall"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="41"/>
+    <x v="2"/>
+    <s v="Students will be able to explain security design principles."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="41"/>
+    <x v="2"/>
+    <s v="Students will be able to apply security principles when they analyze and design projects."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="41"/>
+    <x v="2"/>
+    <s v="Students will be able to implement projects using security primitives."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="41"/>
+    <x v="2"/>
+    <s v="Students will be able to utilize tools for security analysis."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="41"/>
+    <x v="2"/>
+    <s v="Students will be able to evaluate the security of project implementations."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="41"/>
+    <x v="3"/>
+    <s v="This course will cover the following modules:_x000a_• Web Application Security &amp; Practices including SQL injection, cross-site scripting,_x000a_cross-site request forgery, cookies and hidden form fields._x000a_• Implementation Security &amp; Practices including buffer overruns, string formatting issues,_x000a_integer overflows, exceptions, command injection, information leakage, race conditions,_x000a_principle of least privilege._x000a_• Cryptographic Security &amp; Practices including weak passwords, weak cryptography,_x000a_incorrect cryptography._x000a_• Networking Security &amp; Practices including network security overview, secure network_x000a_transmission, name resolution._x000a_• Vulnerability &amp; risk mitigation, vulnerability assessments, &amp; QA testing."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="41"/>
+    <x v="0"/>
+    <s v="Secure Coding Practices"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="41"/>
+    <x v="4"/>
+    <s v="SE 3620"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="41"/>
+    <x v="1"/>
+    <s v="Yr4 - Spring"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="42"/>
+    <x v="2"/>
+    <s v="Students will be able to apply a systematic approach to common engineering problems in the context of their practicum project."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="42"/>
+    <x v="2"/>
+    <s v="Students will demonstrate an ability to apply theories and principles of Software Engineering to problems encountered in industry."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="42"/>
+    <x v="2"/>
+    <s v="Students will demonstrate an ability to exercise and improve time and stress management skills as well as problem-solving skills"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="42"/>
+    <x v="3"/>
+    <s v="This course will consist of a practical software engineering capstone experience. Content covered through the experience will be dependent upon the project assigned to each student. It is expected that each experience will be unique as provided for by a professional sponsor or assigned by the instructor. However, key principles taught throughout the Software Engineering curriculum will be applied to each setting."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="42"/>
+    <x v="0"/>
+    <s v="Software Engineering Practicum I"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="42"/>
+    <x v="4"/>
+    <s v="SE 3450"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="42"/>
+    <x v="4"/>
+    <s v="SE 3620"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="42"/>
+    <x v="1"/>
+    <s v="Yr4 - Fall"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="43"/>
+    <x v="2"/>
+    <s v="Students will be able to apply a systematic approach to common engineering problems in the context of their practicum project."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="43"/>
+    <x v="2"/>
+    <s v="Students will demonstrate an ability to apply theories and principles of Software Engineering to problems encountered in industry."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="43"/>
+    <x v="2"/>
+    <s v="Students will demonstrate an ability to exercise and improve time and stress management skills as well as problem-solving skills."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="43"/>
+    <x v="3"/>
+    <s v="This course will consist of a practical software engineering capstone experience. Content covered through the experience will be dependent upon the project assigned to each student. It is expected that each experience will be unique as provided for by a professional sponsor or assigned by the instructor. However, key principles taught throughout the Software Engineering curriculum will be applied to each setting."/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="43"/>
+    <x v="0"/>
+    <s v="Software Engineering Practicum II"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="43"/>
+    <x v="4"/>
+    <s v="SE 4400"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="43"/>
+    <x v="1"/>
+    <s v="Yr4 - Spring"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{64DE29A7-A041-4FA2-9724-FE192AE510A4}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:H58" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="4">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="9">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="45">
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="13"/>
+        <item x="0"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="14"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="23"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="24"/>
+        <item x="30"/>
+        <item x="15"/>
+        <item x="25"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="36"/>
+        <item x="37"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="40"/>
+        <item x="41"/>
+        <item x="42"/>
+        <item x="43"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="7">
+        <item x="3"/>
+        <item x="5"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="0"/>
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="54">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="9"/>
+    </i>
+    <i r="1">
+      <x v="10"/>
+    </i>
+    <i r="1">
+      <x v="11"/>
+    </i>
+    <i r="1">
+      <x v="12"/>
+    </i>
+    <i r="1">
+      <x v="13"/>
+    </i>
+    <i r="1">
+      <x v="14"/>
+    </i>
+    <i r="1">
+      <x v="21"/>
+    </i>
+    <i r="1">
+      <x v="22"/>
+    </i>
+    <i r="1">
+      <x v="23"/>
+    </i>
+    <i r="1">
+      <x v="24"/>
+    </i>
+    <i r="1">
+      <x v="25"/>
+    </i>
+    <i r="1">
+      <x v="26"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="15"/>
+    </i>
+    <i r="1">
+      <x v="29"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x v="20"/>
+    </i>
+    <i r="1">
+      <x v="27"/>
+    </i>
+    <i r="1">
+      <x v="30"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="16"/>
+    </i>
+    <i r="1">
+      <x v="17"/>
+    </i>
+    <i r="1">
+      <x v="18"/>
+    </i>
+    <i r="1">
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x v="28"/>
+    </i>
+    <i r="1">
+      <x v="31"/>
+    </i>
+    <i r="1">
+      <x v="32"/>
+    </i>
+    <i r="1">
+      <x v="33"/>
+    </i>
+    <i r="1">
+      <x v="34"/>
+    </i>
+    <i r="1">
+      <x v="35"/>
+    </i>
+    <i r="1">
+      <x v="36"/>
+    </i>
+    <i r="1">
+      <x v="37"/>
+    </i>
+    <i r="1">
+      <x v="38"/>
+    </i>
+    <i r="1">
+      <x v="39"/>
+    </i>
+    <i r="1">
+      <x v="40"/>
+    </i>
+    <i r="1">
+      <x v="41"/>
+    </i>
+    <i r="1">
+      <x v="42"/>
+    </i>
+    <i r="1">
+      <x v="43"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="2"/>
+  </colFields>
+  <colItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of ItemText" fld="3" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1108,8 +3079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F90E087-F363-4783-84FA-5A2E6F319782}">
   <dimension ref="A1:D262"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="A98" sqref="A98"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4792,4 +6763,1205 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B67359E-4107-4FFC-A11C-174C4ADEBBB2}">
+  <dimension ref="A3:H58"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>148</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>145</v>
+      </c>
+      <c r="F4" t="s">
+        <v>183</v>
+      </c>
+      <c r="G4" t="s">
+        <v>143</v>
+      </c>
+      <c r="H4" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5">
+        <v>1</v>
+      </c>
+      <c r="G5" s="5">
+        <v>1</v>
+      </c>
+      <c r="H5" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>1020</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5">
+        <v>1</v>
+      </c>
+      <c r="G6" s="5">
+        <v>1</v>
+      </c>
+      <c r="H6" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="5">
+        <v>10</v>
+      </c>
+      <c r="C7" s="5">
+        <v>1</v>
+      </c>
+      <c r="D7" s="5">
+        <v>52</v>
+      </c>
+      <c r="E7" s="5">
+        <v>8</v>
+      </c>
+      <c r="F7" s="5">
+        <v>12</v>
+      </c>
+      <c r="G7" s="5">
+        <v>9</v>
+      </c>
+      <c r="H7" s="5">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
+        <v>1400</v>
+      </c>
+      <c r="B8" s="5">
+        <v>1</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5">
+        <v>3</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5">
+        <v>1</v>
+      </c>
+      <c r="G8" s="5">
+        <v>1</v>
+      </c>
+      <c r="H8" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
+        <v>1405</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5">
+        <v>1</v>
+      </c>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
+        <v>1410</v>
+      </c>
+      <c r="B10" s="5">
+        <v>1</v>
+      </c>
+      <c r="C10" s="5">
+        <v>1</v>
+      </c>
+      <c r="D10" s="5">
+        <v>2</v>
+      </c>
+      <c r="E10" s="5">
+        <v>1</v>
+      </c>
+      <c r="F10" s="5">
+        <v>1</v>
+      </c>
+      <c r="G10" s="5">
+        <v>1</v>
+      </c>
+      <c r="H10" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
+        <v>1415</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5">
+        <v>1</v>
+      </c>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="4">
+        <v>1810</v>
+      </c>
+      <c r="B12" s="5">
+        <v>1</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5">
+        <v>12</v>
+      </c>
+      <c r="E12" s="5">
+        <v>1</v>
+      </c>
+      <c r="F12" s="5">
+        <v>1</v>
+      </c>
+      <c r="G12" s="5">
+        <v>1</v>
+      </c>
+      <c r="H12" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
+        <v>1820</v>
+      </c>
+      <c r="B13" s="5">
+        <v>1</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5">
+        <v>8</v>
+      </c>
+      <c r="E13" s="5">
+        <v>1</v>
+      </c>
+      <c r="F13" s="5">
+        <v>1</v>
+      </c>
+      <c r="G13" s="5">
+        <v>1</v>
+      </c>
+      <c r="H13" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
+        <v>2420</v>
+      </c>
+      <c r="B14" s="5">
+        <v>2</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5">
+        <v>4</v>
+      </c>
+      <c r="E14" s="5">
+        <v>1</v>
+      </c>
+      <c r="F14" s="5">
+        <v>1</v>
+      </c>
+      <c r="G14" s="5">
+        <v>1</v>
+      </c>
+      <c r="H14" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="4">
+        <v>2450</v>
+      </c>
+      <c r="B15" s="5">
+        <v>1</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5">
+        <v>8</v>
+      </c>
+      <c r="E15" s="5">
+        <v>1</v>
+      </c>
+      <c r="F15" s="5">
+        <v>1</v>
+      </c>
+      <c r="G15" s="5">
+        <v>1</v>
+      </c>
+      <c r="H15" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="4">
+        <v>2700</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5">
+        <v>1</v>
+      </c>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="4">
+        <v>2810</v>
+      </c>
+      <c r="B17" s="5">
+        <v>1</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5">
+        <v>2</v>
+      </c>
+      <c r="E17" s="5">
+        <v>1</v>
+      </c>
+      <c r="F17" s="5">
+        <v>1</v>
+      </c>
+      <c r="G17" s="5">
+        <v>1</v>
+      </c>
+      <c r="H17" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="4">
+        <v>2830</v>
+      </c>
+      <c r="B18" s="5">
+        <v>1</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5">
+        <v>5</v>
+      </c>
+      <c r="E18" s="5">
+        <v>1</v>
+      </c>
+      <c r="F18" s="5">
+        <v>1</v>
+      </c>
+      <c r="G18" s="5">
+        <v>1</v>
+      </c>
+      <c r="H18" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="4">
+        <v>2860</v>
+      </c>
+      <c r="B19" s="5">
+        <v>1</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5">
+        <v>8</v>
+      </c>
+      <c r="E19" s="5">
+        <v>1</v>
+      </c>
+      <c r="F19" s="5">
+        <v>1</v>
+      </c>
+      <c r="G19" s="5">
+        <v>1</v>
+      </c>
+      <c r="H19" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5">
+        <v>2</v>
+      </c>
+      <c r="F20" s="5">
+        <v>3</v>
+      </c>
+      <c r="G20" s="5">
+        <v>3</v>
+      </c>
+      <c r="H20" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="4">
+        <v>1010</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5">
+        <v>1</v>
+      </c>
+      <c r="G21" s="5">
+        <v>1</v>
+      </c>
+      <c r="H21" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="4">
+        <v>2010</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5">
+        <v>1</v>
+      </c>
+      <c r="F22" s="5">
+        <v>1</v>
+      </c>
+      <c r="G22" s="5">
+        <v>1</v>
+      </c>
+      <c r="H22" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="4">
+        <v>3260</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5">
+        <v>1</v>
+      </c>
+      <c r="F23" s="5">
+        <v>1</v>
+      </c>
+      <c r="G23" s="5">
+        <v>1</v>
+      </c>
+      <c r="H23" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5">
+        <v>4</v>
+      </c>
+      <c r="G24" s="5">
+        <v>5</v>
+      </c>
+      <c r="H24" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="4">
+        <v>1</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5">
+        <v>1</v>
+      </c>
+      <c r="H25" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="4">
+        <v>2</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5">
+        <v>1</v>
+      </c>
+      <c r="G26" s="5">
+        <v>1</v>
+      </c>
+      <c r="H26" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="4">
+        <v>3</v>
+      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5">
+        <v>1</v>
+      </c>
+      <c r="G27" s="5">
+        <v>1</v>
+      </c>
+      <c r="H27" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="4">
+        <v>4</v>
+      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5">
+        <v>1</v>
+      </c>
+      <c r="G28" s="5">
+        <v>1</v>
+      </c>
+      <c r="H28" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="4">
+        <v>5</v>
+      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5">
+        <v>1</v>
+      </c>
+      <c r="G29" s="5">
+        <v>1</v>
+      </c>
+      <c r="H29" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5">
+        <v>1</v>
+      </c>
+      <c r="G30" s="5">
+        <v>1</v>
+      </c>
+      <c r="H30" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="4">
+        <v>1</v>
+      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5">
+        <v>1</v>
+      </c>
+      <c r="G31" s="5">
+        <v>1</v>
+      </c>
+      <c r="H31" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5">
+        <v>4</v>
+      </c>
+      <c r="F32" s="5">
+        <v>5</v>
+      </c>
+      <c r="G32" s="5">
+        <v>5</v>
+      </c>
+      <c r="H32" s="5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="4">
+        <v>1210</v>
+      </c>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5">
+        <v>1</v>
+      </c>
+      <c r="G33" s="5">
+        <v>2</v>
+      </c>
+      <c r="H33" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="4">
+        <v>1220</v>
+      </c>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5">
+        <v>1</v>
+      </c>
+      <c r="F34" s="5">
+        <v>1</v>
+      </c>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="4">
+        <v>2270</v>
+      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5">
+        <v>1</v>
+      </c>
+      <c r="F35" s="5">
+        <v>1</v>
+      </c>
+      <c r="G35" s="5">
+        <v>1</v>
+      </c>
+      <c r="H35" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" s="4">
+        <v>3040</v>
+      </c>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5">
+        <v>1</v>
+      </c>
+      <c r="F36" s="5">
+        <v>1</v>
+      </c>
+      <c r="G36" s="5">
+        <v>1</v>
+      </c>
+      <c r="H36" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="4">
+        <v>3310</v>
+      </c>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5">
+        <v>1</v>
+      </c>
+      <c r="F37" s="5">
+        <v>1</v>
+      </c>
+      <c r="G37" s="5">
+        <v>1</v>
+      </c>
+      <c r="H37" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5">
+        <v>1</v>
+      </c>
+      <c r="F38" s="5">
+        <v>4</v>
+      </c>
+      <c r="G38" s="5">
+        <v>4</v>
+      </c>
+      <c r="H38" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" s="4">
+        <v>2210</v>
+      </c>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5">
+        <v>1</v>
+      </c>
+      <c r="G39" s="5">
+        <v>1</v>
+      </c>
+      <c r="H39" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40" s="4">
+        <v>2215</v>
+      </c>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5">
+        <v>1</v>
+      </c>
+      <c r="G40" s="5">
+        <v>1</v>
+      </c>
+      <c r="H40" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41" s="4">
+        <v>2220</v>
+      </c>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5">
+        <v>1</v>
+      </c>
+      <c r="F41" s="5">
+        <v>1</v>
+      </c>
+      <c r="G41" s="5">
+        <v>1</v>
+      </c>
+      <c r="H41" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" s="4">
+        <v>2225</v>
+      </c>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5">
+        <v>1</v>
+      </c>
+      <c r="G42" s="5">
+        <v>1</v>
+      </c>
+      <c r="H42" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B43" s="5">
+        <v>14</v>
+      </c>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5">
+        <v>65</v>
+      </c>
+      <c r="E43" s="5">
+        <v>18</v>
+      </c>
+      <c r="F43" s="5">
+        <v>14</v>
+      </c>
+      <c r="G43" s="5">
+        <v>14</v>
+      </c>
+      <c r="H43" s="5">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44" s="4">
+        <v>3250</v>
+      </c>
+      <c r="B44" s="5">
+        <v>1</v>
+      </c>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5">
+        <v>3</v>
+      </c>
+      <c r="E44" s="5">
+        <v>1</v>
+      </c>
+      <c r="F44" s="5">
+        <v>1</v>
+      </c>
+      <c r="G44" s="5">
+        <v>1</v>
+      </c>
+      <c r="H44" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45" s="4">
+        <v>3410</v>
+      </c>
+      <c r="B45" s="5">
+        <v>1</v>
+      </c>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5">
+        <v>10</v>
+      </c>
+      <c r="E45" s="5">
+        <v>1</v>
+      </c>
+      <c r="F45" s="5">
+        <v>1</v>
+      </c>
+      <c r="G45" s="5">
+        <v>1</v>
+      </c>
+      <c r="H45" s="5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46" s="4">
+        <v>3450</v>
+      </c>
+      <c r="B46" s="5">
+        <v>1</v>
+      </c>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5">
+        <v>3</v>
+      </c>
+      <c r="E46" s="5">
+        <v>1</v>
+      </c>
+      <c r="F46" s="5">
+        <v>1</v>
+      </c>
+      <c r="G46" s="5">
+        <v>1</v>
+      </c>
+      <c r="H46" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47" s="4">
+        <v>3520</v>
+      </c>
+      <c r="B47" s="5">
+        <v>1</v>
+      </c>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5">
+        <v>8</v>
+      </c>
+      <c r="E47" s="5">
+        <v>1</v>
+      </c>
+      <c r="F47" s="5">
+        <v>1</v>
+      </c>
+      <c r="G47" s="5">
+        <v>1</v>
+      </c>
+      <c r="H47" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48" s="4">
+        <v>3620</v>
+      </c>
+      <c r="B48" s="5">
+        <v>1</v>
+      </c>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5">
+        <v>5</v>
+      </c>
+      <c r="E48" s="5">
+        <v>2</v>
+      </c>
+      <c r="F48" s="5">
+        <v>1</v>
+      </c>
+      <c r="G48" s="5">
+        <v>1</v>
+      </c>
+      <c r="H48" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A49" s="4">
+        <v>3630</v>
+      </c>
+      <c r="B49" s="5">
+        <v>1</v>
+      </c>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5">
+        <v>2</v>
+      </c>
+      <c r="E49" s="5">
+        <v>1</v>
+      </c>
+      <c r="F49" s="5">
+        <v>1</v>
+      </c>
+      <c r="G49" s="5">
+        <v>1</v>
+      </c>
+      <c r="H49" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A50" s="4">
+        <v>4120</v>
+      </c>
+      <c r="B50" s="5">
+        <v>1</v>
+      </c>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5">
+        <v>6</v>
+      </c>
+      <c r="E50" s="5">
+        <v>1</v>
+      </c>
+      <c r="F50" s="5">
+        <v>1</v>
+      </c>
+      <c r="G50" s="5">
+        <v>1</v>
+      </c>
+      <c r="H50" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51" s="4">
+        <v>4140</v>
+      </c>
+      <c r="B51" s="5">
+        <v>1</v>
+      </c>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5">
+        <v>6</v>
+      </c>
+      <c r="E51" s="5">
+        <v>1</v>
+      </c>
+      <c r="F51" s="5">
+        <v>1</v>
+      </c>
+      <c r="G51" s="5">
+        <v>1</v>
+      </c>
+      <c r="H51" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A52" s="4">
+        <v>4220</v>
+      </c>
+      <c r="B52" s="5">
+        <v>1</v>
+      </c>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5">
+        <v>3</v>
+      </c>
+      <c r="E52" s="5">
+        <v>2</v>
+      </c>
+      <c r="F52" s="5">
+        <v>1</v>
+      </c>
+      <c r="G52" s="5">
+        <v>1</v>
+      </c>
+      <c r="H52" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A53" s="4">
+        <v>4230</v>
+      </c>
+      <c r="B53" s="5">
+        <v>1</v>
+      </c>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5">
+        <v>4</v>
+      </c>
+      <c r="E53" s="5">
+        <v>2</v>
+      </c>
+      <c r="F53" s="5">
+        <v>1</v>
+      </c>
+      <c r="G53" s="5">
+        <v>1</v>
+      </c>
+      <c r="H53" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A54" s="4">
+        <v>4320</v>
+      </c>
+      <c r="B54" s="5">
+        <v>1</v>
+      </c>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5">
+        <v>4</v>
+      </c>
+      <c r="E54" s="5">
+        <v>1</v>
+      </c>
+      <c r="F54" s="5">
+        <v>1</v>
+      </c>
+      <c r="G54" s="5">
+        <v>1</v>
+      </c>
+      <c r="H54" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A55" s="4">
+        <v>4340</v>
+      </c>
+      <c r="B55" s="5">
+        <v>1</v>
+      </c>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5">
+        <v>5</v>
+      </c>
+      <c r="E55" s="5">
+        <v>1</v>
+      </c>
+      <c r="F55" s="5">
+        <v>1</v>
+      </c>
+      <c r="G55" s="5">
+        <v>1</v>
+      </c>
+      <c r="H55" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A56" s="4">
+        <v>4400</v>
+      </c>
+      <c r="B56" s="5">
+        <v>1</v>
+      </c>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5">
+        <v>3</v>
+      </c>
+      <c r="E56" s="5">
+        <v>2</v>
+      </c>
+      <c r="F56" s="5">
+        <v>1</v>
+      </c>
+      <c r="G56" s="5">
+        <v>1</v>
+      </c>
+      <c r="H56" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A57" s="4">
+        <v>4450</v>
+      </c>
+      <c r="B57" s="5">
+        <v>1</v>
+      </c>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5">
+        <v>3</v>
+      </c>
+      <c r="E57" s="5">
+        <v>1</v>
+      </c>
+      <c r="F57" s="5">
+        <v>1</v>
+      </c>
+      <c r="G57" s="5">
+        <v>1</v>
+      </c>
+      <c r="H57" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A58" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="B58" s="5">
+        <v>24</v>
+      </c>
+      <c r="C58" s="5">
+        <v>1</v>
+      </c>
+      <c r="D58" s="5">
+        <v>117</v>
+      </c>
+      <c r="E58" s="5">
+        <v>33</v>
+      </c>
+      <c r="F58" s="5">
+        <v>44</v>
+      </c>
+      <c r="G58" s="5">
+        <v>42</v>
+      </c>
+      <c r="H58" s="5">
+        <v>261</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>